<commit_message>
add google maps service
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Фамилия</t>
   </si>
@@ -63,20 +63,25 @@
     <t>Юрьевич</t>
   </si>
   <si>
-    <t>http://habrastorage.org/storage1/cf1a57bd/e7cc2b34/b9d6fc1d/0a19729c.jpg 
- http://www.featuredpix.com/uploads/0/91_500x500.jpg</t>
-  </si>
-  <si>
     <t>https://img.drive.ru/i/3/56936ef595a656dfb000002c.jpg</t>
   </si>
   <si>
     <t>Пашкевич</t>
+  </si>
+  <si>
+    <t>Минск</t>
+  </si>
+  <si>
+    <t>г.ЖлобинБеларусь</t>
+  </si>
+  <si>
+    <t>http://habrastorage.org/storage1/cf1a57bd/e7cc2b34/b9d6fc1d/0a19729c.jpg http://www.featuredpix.com/uploads/0/91_500x500.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -123,8 +128,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -394,7 +399,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -404,8 +409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,8 +472,8 @@
       <c r="D2" s="1">
         <v>32984</v>
       </c>
-      <c r="E2" s="1">
-        <v>32984</v>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="G2" s="1">
         <v>32984</v>
@@ -483,12 +488,12 @@
         <v>123</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -499,8 +504,8 @@
       <c r="D3" s="1">
         <v>32984</v>
       </c>
-      <c r="E3" s="1">
-        <v>32984</v>
+      <c r="E3" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="G3" s="1">
         <v>32984</v>
@@ -515,12 +520,12 @@
         <v>123</v>
       </c>
       <c r="K3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1" display="http://habrastorage.org/storage1/cf1a57bd/e7cc2b34/b9d6fc1d/0a19729c.jpg  "/>
+    <hyperlink ref="K2" r:id="rId1" display="http://habrastorage.org/storage1/cf1a57bd/e7cc2b34/b9d6fc1d/0a19729c.jpghttp://www.featuredpix.com/uploads/0/91_500x500.jpg"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>